<commit_message>
Updated the Course.java and CourseReader
Updated the Course.java and CourseReader
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/CurriculumSummary.xlsx
+++ b/On-Call-Tracker/src/inputs/CurriculumSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmac\My Drive\Sync\My Documents\My Teaching\Courses - Ugrad\CS2043\2022-23\Project\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E950AA8-334A-444A-9547-4C739BED6628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B6AF98-0068-3B42-9D8C-2330D128A16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5FF850C6-C8B3-9244-B09D-6F4F2E2962B0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{5FF850C6-C8B3-9244-B09D-6F4F2E2962B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="439">
   <si>
     <t>Technological Education</t>
   </si>
@@ -972,12 +972,6 @@
   </si>
   <si>
     <t>IDC4O/IDP4O</t>
-  </si>
-  <si>
-    <t>Cooperative Education Linked to a Related Course (or Courses)</t>
-  </si>
-  <si>
-    <t>Secondary</t>
   </si>
   <si>
     <t>DCO3O</t>
@@ -1725,30 +1719,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD343853-F42A-4BAC-AADE-8C0EB2B59FFB}">
-  <dimension ref="A1:E298"/>
+  <dimension ref="A1:E297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.375" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>20</v>
@@ -1757,7 +1751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1774,7 +1768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1791,7 +1785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1808,7 +1802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1825,7 +1819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1842,7 +1836,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1859,7 +1853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1876,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1893,7 +1887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1910,7 +1904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1927,7 +1921,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1944,7 +1938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1961,7 +1955,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1978,7 +1972,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1995,7 +1989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2012,7 +2006,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2029,7 +2023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2063,7 +2057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2080,7 +2074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2097,7 +2091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2114,7 +2108,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2131,7 +2125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2148,7 +2142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2182,7 +2176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2199,7 +2193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2216,7 +2210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2250,7 +2244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2267,7 +2261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2284,7 +2278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2301,7 +2295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2318,15 +2312,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C35" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D35" s="1">
         <v>11</v>
@@ -2335,15 +2329,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D36" s="1">
         <v>11</v>
@@ -2352,15 +2346,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C37" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D37" s="1">
         <v>12</v>
@@ -2369,15 +2363,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D38" s="1">
         <v>12</v>
@@ -2386,15 +2380,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C39" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D39" s="1">
         <v>12</v>
@@ -2403,15 +2397,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C40" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D40" s="1">
         <v>12</v>
@@ -2420,15 +2414,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C41" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D41" s="1">
         <v>9</v>
@@ -2437,15 +2431,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C42" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D42" s="1">
         <v>10</v>
@@ -2454,15 +2448,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C43" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D43" s="1">
         <v>11</v>
@@ -2471,15 +2465,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C44" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D44" s="1">
         <v>11</v>
@@ -2488,15 +2482,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C45" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D45" s="1">
         <v>12</v>
@@ -2505,15 +2499,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C46" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D46" s="1">
         <v>11</v>
@@ -2522,15 +2516,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C47" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D47" s="1">
         <v>11</v>
@@ -2539,15 +2533,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C48" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D48" s="1">
         <v>12</v>
@@ -2556,15 +2550,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C49" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D49" s="1">
         <v>12</v>
@@ -2573,15 +2567,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C50" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D50" s="1">
         <v>11</v>
@@ -2590,15 +2584,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C51" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D51" s="1">
         <v>9</v>
@@ -2607,15 +2601,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C52" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D52" s="1">
         <v>10</v>
@@ -2624,15 +2618,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C53" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D53" s="1">
         <v>12</v>
@@ -2641,15 +2635,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C54" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D54" s="1">
         <v>12</v>
@@ -2658,15 +2652,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C55" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D55" s="1">
         <v>9</v>
@@ -2675,15 +2669,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C56" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D56" s="1">
         <v>11</v>
@@ -2692,15 +2686,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C57" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D57" s="1">
         <v>11</v>
@@ -2709,15 +2703,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C58" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D58" s="1">
         <v>11</v>
@@ -2726,15 +2720,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C59" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D59" s="1">
         <v>12</v>
@@ -2743,15 +2737,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C60" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D60" s="1">
         <v>12</v>
@@ -2760,15 +2754,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C61" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D61" s="1">
         <v>12</v>
@@ -2777,15 +2771,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C62" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D62" s="1">
         <v>11</v>
@@ -2794,15 +2788,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C63" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D63" s="1">
         <v>12</v>
@@ -2811,15 +2805,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C64" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D64" s="1">
         <v>12</v>
@@ -2828,15 +2822,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C65" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D65" s="1">
         <v>12</v>
@@ -2845,15 +2839,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D66" s="1">
         <v>11</v>
@@ -2862,15 +2856,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C67" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D67" s="1">
         <v>10</v>
@@ -2879,15 +2873,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C68" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D68" s="1">
         <v>10</v>
@@ -2896,15 +2890,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C69" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D69" s="1">
         <v>11</v>
@@ -2913,15 +2907,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C70" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D70" s="1">
         <v>12</v>
@@ -2930,15 +2924,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C71" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D71" s="1">
         <v>12</v>
@@ -2947,15 +2941,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C72" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D72" s="1">
         <v>11</v>
@@ -2964,15 +2958,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C73" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D73" s="1">
         <v>10</v>
@@ -2981,15 +2975,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C74" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D74" s="1">
         <v>11</v>
@@ -2998,15 +2992,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C75" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D75" s="1">
         <v>12</v>
@@ -3015,15 +3009,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C76" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D76" s="1">
         <v>12</v>
@@ -3032,15 +3026,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C77" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D77" s="1">
         <v>12</v>
@@ -3049,15 +3043,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C78" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D78" s="1">
         <v>12</v>
@@ -3066,15 +3060,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C79" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D79" s="1">
         <v>11</v>
@@ -3083,15 +3077,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C80" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D80" s="1">
         <v>12</v>
@@ -3100,15 +3094,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C81" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D81" s="1">
         <v>12</v>
@@ -3117,15 +3111,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C82" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D82" s="1">
         <v>11</v>
@@ -3134,15 +3128,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C83" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D83" s="1">
         <v>11</v>
@@ -3151,15 +3145,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>4</v>
       </c>
       <c r="B84" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C84" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D84" s="1">
         <v>11</v>
@@ -3168,15 +3162,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C85" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D85" s="1">
         <v>12</v>
@@ -3185,15 +3179,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C86" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D86" s="1">
         <v>11</v>
@@ -3202,7 +3196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -3219,7 +3213,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -3236,7 +3230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -3253,7 +3247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -3270,7 +3264,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -3287,7 +3281,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -3304,7 +3298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -3321,7 +3315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -3338,7 +3332,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -3355,7 +3349,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -3372,7 +3366,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -3389,7 +3383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -3406,7 +3400,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -3423,7 +3417,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -3440,7 +3434,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -3457,7 +3451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -3474,7 +3468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -3491,7 +3485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -3508,7 +3502,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -3525,7 +3519,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -3542,7 +3536,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -3559,7 +3553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -3576,7 +3570,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3587,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -3610,7 +3604,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -3627,7 +3621,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -3644,7 +3638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -3661,7 +3655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -3678,7 +3672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>9</v>
       </c>
@@ -3695,7 +3689,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>9</v>
       </c>
@@ -3712,7 +3706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>9</v>
       </c>
@@ -3729,7 +3723,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -3746,7 +3740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3763,7 +3757,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -3780,7 +3774,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>9</v>
       </c>
@@ -3797,7 +3791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -3814,7 +3808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -3831,7 +3825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -3848,7 +3842,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -3865,7 +3859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -3882,7 +3876,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -3899,7 +3893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -3916,7 +3910,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -3933,7 +3927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -3950,7 +3944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -3967,7 +3961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>2</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>2</v>
       </c>
@@ -4001,7 +3995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -4018,7 +4012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -4035,7 +4029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>2</v>
       </c>
@@ -4052,7 +4046,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -4069,7 +4063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -4086,7 +4080,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -4103,15 +4097,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>3</v>
       </c>
       <c r="B140" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C140" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D140" s="1">
         <v>12</v>
@@ -4120,15 +4114,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>3</v>
       </c>
       <c r="B141" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C141" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D141" s="1">
         <v>12</v>
@@ -4137,15 +4131,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C142" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D142" s="1">
         <v>11</v>
@@ -4154,15 +4148,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>3</v>
       </c>
       <c r="B143" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C143" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D143" s="1">
         <v>11</v>
@@ -4171,15 +4165,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>3</v>
       </c>
       <c r="B144" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C144" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D144" s="1">
         <v>12</v>
@@ -4188,15 +4182,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>3</v>
       </c>
       <c r="B145" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C145" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D145" s="1">
         <v>9</v>
@@ -4205,15 +4199,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>3</v>
       </c>
       <c r="B146" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C146" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D146" s="1">
         <v>10</v>
@@ -4222,15 +4216,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>3</v>
       </c>
       <c r="B147" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C147" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D147" s="1">
         <v>11</v>
@@ -4239,15 +4233,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>3</v>
       </c>
       <c r="B148" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C148" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D148" s="1">
         <v>12</v>
@@ -4256,15 +4250,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>3</v>
       </c>
       <c r="B149" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C149" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D149" s="1">
         <v>12</v>
@@ -4273,15 +4267,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>3</v>
       </c>
       <c r="B150" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C150" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D150" s="1">
         <v>12</v>
@@ -4290,15 +4284,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>3</v>
       </c>
       <c r="B151" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C151" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D151" s="1">
         <v>9</v>
@@ -4307,15 +4301,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>3</v>
       </c>
       <c r="B152" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C152" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D152" s="1">
         <v>10</v>
@@ -4324,15 +4318,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>3</v>
       </c>
       <c r="B153" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C153" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D153" s="1">
         <v>12</v>
@@ -4341,15 +4335,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>3</v>
       </c>
       <c r="B154" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C154" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D154" s="1">
         <v>11</v>
@@ -4358,15 +4352,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>3</v>
       </c>
       <c r="B155" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C155" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D155" s="1">
         <v>12</v>
@@ -4375,15 +4369,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>3</v>
       </c>
       <c r="B156" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C156" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D156" s="1">
         <v>11</v>
@@ -4392,15 +4386,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>3</v>
       </c>
       <c r="B157" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C157" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D157" s="1">
         <v>10</v>
@@ -4409,15 +4403,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>3</v>
       </c>
       <c r="B158" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C158" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D158" s="1">
         <v>11</v>
@@ -4426,15 +4420,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>3</v>
       </c>
       <c r="B159" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C159" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D159" s="1">
         <v>12</v>
@@ -4443,15 +4437,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>3</v>
       </c>
       <c r="B160" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C160" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D160" s="1">
         <v>11</v>
@@ -4460,15 +4454,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>3</v>
       </c>
       <c r="B161" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C161" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D161" s="1">
         <v>11</v>
@@ -4477,15 +4471,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>3</v>
       </c>
       <c r="B162" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C162" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D162" s="1">
         <v>11</v>
@@ -4494,15 +4488,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>3</v>
       </c>
       <c r="B163" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C163" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D163" s="1">
         <v>12</v>
@@ -4511,15 +4505,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C164" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D164" s="1">
         <v>12</v>
@@ -4528,15 +4522,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>3</v>
       </c>
       <c r="B165" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C165" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D165" s="1">
         <v>11</v>
@@ -4545,15 +4539,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>3</v>
       </c>
       <c r="B166" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C166" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D166" s="1">
         <v>12</v>
@@ -4562,15 +4556,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>3</v>
       </c>
       <c r="B167" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C167" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D167" s="1">
         <v>11</v>
@@ -4579,15 +4573,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>3</v>
       </c>
       <c r="B168" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C168" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D168" s="1">
         <v>11</v>
@@ -4596,15 +4590,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>3</v>
       </c>
       <c r="B169" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C169" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D169" s="1">
         <v>11</v>
@@ -4613,15 +4607,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>3</v>
       </c>
       <c r="B170" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C170" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D170" s="1">
         <v>11</v>
@@ -4630,15 +4624,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>3</v>
       </c>
       <c r="B171" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C171" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D171" s="1">
         <v>12</v>
@@ -4647,15 +4641,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>7</v>
       </c>
       <c r="B172" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C172" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D172" s="1">
         <v>10</v>
@@ -4664,15 +4658,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>7</v>
       </c>
       <c r="B173" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C173" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D173" s="1">
         <v>11</v>
@@ -4681,15 +4675,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>7</v>
       </c>
       <c r="B174" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C174" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D174" s="1">
         <v>11</v>
@@ -4698,15 +4692,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>7</v>
       </c>
       <c r="B175" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C175" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D175" s="1">
         <v>12</v>
@@ -4715,15 +4709,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>7</v>
       </c>
       <c r="B176" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C176" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D176" s="1">
         <v>12</v>
@@ -4732,7 +4726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>17</v>
       </c>
@@ -4749,7 +4743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>17</v>
       </c>
@@ -4766,7 +4760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>17</v>
       </c>
@@ -4783,12 +4777,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>8</v>
       </c>
       <c r="B180" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C180" t="s">
         <v>8</v>
@@ -4800,15 +4794,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>6</v>
       </c>
       <c r="B181" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C181" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>291</v>
@@ -4817,15 +4811,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>6</v>
       </c>
       <c r="B182" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C182" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>291</v>
@@ -4834,15 +4828,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>6</v>
       </c>
       <c r="B183" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C183" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>293</v>
@@ -4851,15 +4845,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>6</v>
       </c>
       <c r="B184" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C184" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>293</v>
@@ -4868,15 +4862,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>6</v>
       </c>
       <c r="B185" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C185" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>295</v>
@@ -4885,15 +4879,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>6</v>
       </c>
       <c r="B186" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C186" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>295</v>
@@ -4902,7 +4896,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>15</v>
       </c>
@@ -4919,7 +4913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>15</v>
       </c>
@@ -4936,7 +4930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>15</v>
       </c>
@@ -4953,7 +4947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>15</v>
       </c>
@@ -4970,7 +4964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>15</v>
       </c>
@@ -4987,15 +4981,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>6</v>
       </c>
       <c r="B192" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C192" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>291</v>
@@ -5004,15 +4998,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>6</v>
       </c>
       <c r="B193" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C193" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>293</v>
@@ -5021,15 +5015,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>6</v>
       </c>
       <c r="B194" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C194" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>295</v>
@@ -5038,15 +5032,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>6</v>
       </c>
       <c r="B195" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C195" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D195" s="1">
         <v>12</v>
@@ -5055,7 +5049,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>12</v>
       </c>
@@ -5072,7 +5066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>12</v>
       </c>
@@ -5089,7 +5083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>12</v>
       </c>
@@ -5106,7 +5100,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>12</v>
       </c>
@@ -5123,7 +5117,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>12</v>
       </c>
@@ -5140,7 +5134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>12</v>
       </c>
@@ -5157,7 +5151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>12</v>
       </c>
@@ -5174,7 +5168,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>12</v>
       </c>
@@ -5191,7 +5185,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>12</v>
       </c>
@@ -5208,7 +5202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>12</v>
       </c>
@@ -5225,7 +5219,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>12</v>
       </c>
@@ -5242,7 +5236,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>12</v>
       </c>
@@ -5259,7 +5253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>12</v>
       </c>
@@ -5276,7 +5270,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>13</v>
       </c>
@@ -5293,7 +5287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>13</v>
       </c>
@@ -5310,7 +5304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>13</v>
       </c>
@@ -5327,7 +5321,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>13</v>
       </c>
@@ -5344,7 +5338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>13</v>
       </c>
@@ -5361,7 +5355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>13</v>
       </c>
@@ -5378,7 +5372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>13</v>
       </c>
@@ -5395,7 +5389,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>13</v>
       </c>
@@ -5412,7 +5406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>13</v>
       </c>
@@ -5429,7 +5423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>13</v>
       </c>
@@ -5446,7 +5440,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>10</v>
       </c>
@@ -5463,7 +5457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>14</v>
       </c>
@@ -5480,7 +5474,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>14</v>
       </c>
@@ -5497,7 +5491,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>14</v>
       </c>
@@ -5514,7 +5508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>14</v>
       </c>
@@ -5531,7 +5525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>14</v>
       </c>
@@ -5548,7 +5542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>14</v>
       </c>
@@ -5565,7 +5559,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>14</v>
       </c>
@@ -5582,7 +5576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>11</v>
       </c>
@@ -5599,7 +5593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>11</v>
       </c>
@@ -5616,7 +5610,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>11</v>
       </c>
@@ -5633,7 +5627,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>11</v>
       </c>
@@ -5650,7 +5644,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>11</v>
       </c>
@@ -5667,7 +5661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>11</v>
       </c>
@@ -5684,7 +5678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>11</v>
       </c>
@@ -5701,7 +5695,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>11</v>
       </c>
@@ -5718,7 +5712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>11</v>
       </c>
@@ -5735,7 +5729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>11</v>
       </c>
@@ -5752,7 +5746,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>11</v>
       </c>
@@ -5769,7 +5763,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>11</v>
       </c>
@@ -5786,7 +5780,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>11</v>
       </c>
@@ -5803,7 +5797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>11</v>
       </c>
@@ -5820,7 +5814,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>11</v>
       </c>
@@ -5837,7 +5831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -5854,7 +5848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -5871,7 +5865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -5888,7 +5882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -5905,7 +5899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -5922,7 +5916,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -5939,7 +5933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -5956,7 +5950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -5973,7 +5967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -5990,7 +5984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -6007,7 +6001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -6024,7 +6018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -6041,7 +6035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>0</v>
       </c>
@@ -6058,7 +6052,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -6075,7 +6069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>0</v>
       </c>
@@ -6092,7 +6086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -6109,7 +6103,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -6126,7 +6120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>0</v>
       </c>
@@ -6143,7 +6137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>0</v>
       </c>
@@ -6160,7 +6154,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>0</v>
       </c>
@@ -6177,7 +6171,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -6194,7 +6188,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>0</v>
       </c>
@@ -6211,7 +6205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>0</v>
       </c>
@@ -6228,7 +6222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>0</v>
       </c>
@@ -6245,7 +6239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>0</v>
       </c>
@@ -6262,7 +6256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -6279,7 +6273,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>0</v>
       </c>
@@ -6296,7 +6290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>0</v>
       </c>
@@ -6313,7 +6307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>0</v>
       </c>
@@ -6330,7 +6324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>0</v>
       </c>
@@ -6347,7 +6341,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>0</v>
       </c>
@@ -6364,7 +6358,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>0</v>
       </c>
@@ -6381,7 +6375,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>0</v>
       </c>
@@ -6398,7 +6392,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>0</v>
       </c>
@@ -6415,7 +6409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>0</v>
       </c>
@@ -6432,7 +6426,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>0</v>
       </c>
@@ -6449,7 +6443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>0</v>
       </c>
@@ -6466,7 +6460,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>0</v>
       </c>
@@ -6483,7 +6477,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>0</v>
       </c>
@@ -6500,7 +6494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>0</v>
       </c>
@@ -6517,7 +6511,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>0</v>
       </c>
@@ -6534,7 +6528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>0</v>
       </c>
@@ -6551,7 +6545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>0</v>
       </c>
@@ -6568,7 +6562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>0</v>
       </c>
@@ -6585,7 +6579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>0</v>
       </c>
@@ -6602,7 +6596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>0</v>
       </c>
@@ -6619,7 +6613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>0</v>
       </c>
@@ -6636,7 +6630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>0</v>
       </c>
@@ -6653,7 +6647,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>0</v>
       </c>
@@ -6670,7 +6664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>0</v>
       </c>
@@ -6687,7 +6681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>0</v>
       </c>
@@ -6704,7 +6698,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>0</v>
       </c>
@@ -6721,7 +6715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>0</v>
       </c>
@@ -6738,7 +6732,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>0</v>
       </c>
@@ -6755,7 +6749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>0</v>
       </c>
@@ -6772,7 +6766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>0</v>
       </c>
@@ -6787,17 +6781,6 @@
       </c>
       <c r="E297" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>18</v>
-      </c>
-      <c r="C298" t="s">
-        <v>312</v>
-      </c>
-      <c r="D298" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -6807,21 +6790,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C1944CEC9F89E1428E52E95D177456E2" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a652b8930afa24269c2c8d1f2c806de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="88dc6573-aa6b-4fe6-87e0-c2ee6cd75f6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="26f26de8e71a57434d6d87bd8c325111" ns2:_="">
     <xsd:import namespace="88dc6573-aa6b-4fe6-87e0-c2ee6cd75f6c"/>
@@ -6953,24 +6921,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24D0760A-1649-4969-9A76-EEAEDE41DD12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1CD920B-4543-48AC-ABE0-80AF91105465}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50C0585C-1139-4444-BB6C-84070433229F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6986,4 +6952,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1CD920B-4543-48AC-ABE0-80AF91105465}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24D0760A-1649-4969-9A76-EEAEDE41DD12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>